<commit_message>
fix: data classes & tests
</commit_message>
<xml_diff>
--- a/data/sounds.xlsx
+++ b/data/sounds.xlsx
@@ -91,7 +91,7 @@
     <t>Velars</t>
   </si>
   <si>
-    <t>HaäāǟAeɛēEiɨīIoöōȫOuüūǖUʌVəɔɵɞɪɯʉɤɘʊʋɐɑɒɜъЪаАиИоОуУыЫьЬэЭæœʸˤʰʷ</t>
+    <t>HAEIOUaeiouÀÁÂÃÄÅÆÈÉÊËÌÍÎÏÒÓÔÕÖØÙÚÛÜàáâãäåæèéêëìíîïòóôõöøùúûüĀāĂăĄąĒēĔĕĖėĘęĚěĨĩĪīĬĭĮįİıŌōŎŏŐőŒœŨũŪūŬŭŮůŰűŲųƎƏƐƗƖƜƟơƠƯưƱƲǍǎǏǐǑǒǓǔǕǖǗǘǙǚǛǜǝǞǟǠǡǢǣǪǫǬǭǺǻǼǽǾǿȀȁȂȃȄȅȆȇȈȉȊȋȌȍȎȏȔȕȖȗȢȣȦȧȨȩȪȫȬȭȮȯȰȱȺɄɅɆɇɐɑɒɏɎɔɘəɚɛɜɝɞɤɨɩɪɯɰɵɶɷʉʊʌʏʚαεηιουωϊϋόύώάέήίЀЁЍАЕИОУЫЭЮЯаеиоуыэюяѐёєіїѝӐӑӒӓӔӕӖӗӘәӚӛӢӣӤӥӦӧӨөӪӫӬӭӮӯӰӱӸӹᴀᴁᴂᴇᴈᴉᴏᴐᴑᴒᴓᴔᴕᴖᴗᴜᴝᴞᴟᴥᴧᵫᵾᵿᵼᵻᶏᶐᶒᶓᶔᶕᶖᶗᶙḀḁḔḕḖḗḘḙḚḛḜḝḬḭḮḯṌṍṎṏṐṑṒṓṲṳṴṵṶṷṸṹṺṻẚẙẠạẢảẤấẦầẨẩẪẫẬậẮắẰằẲẳẴẵẶặẸẹẺẻẼẽẾếỀềỂểỄễỆệỈỉỊịỌọỎỏỐốỒồổỔỖỗỘộỚớỜờỞởỠỡỢợỤụỦủỨứỪừỬửỮữỰựὰάὲέὴήὶίὸόὺύὼώⱯꝊꝋꝌꝍꝎꝏꞶꞷꞜꞝ</t>
   </si>
   <si>
     <t>Vowels and features</t>
@@ -1265,9 +1265,7 @@
   <cols>
     <col min="1" max="1" width="84.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.1719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="1" customWidth="1"/>
+    <col min="3" max="5" width="9.17188" style="1" customWidth="1"/>
     <col min="6" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>